<commit_message>
Fix pipeline for researchers: venv, async, httpx, coding scheme, sample data
- README: venv setup, run_web.sh, troubleshooting for pip/flask errors
- requirements: flask[async], httpx<0.28 for OpenAI compatibility
- run_pipeline: optional simplified_name, human_codes; derive from display_name
- web_interface: fix sys.path order, sample data fallback
- scripts/run_web.sh: one-command web app start
- prompt.txt: fix JSON syntax (missing comma)
- sample data: single entry (Moodle course design)

Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/data/training_data_sample.xlsx
+++ b/data/training_data_sample.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -17,13 +17,16 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -34,7 +37,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,12 +45,21 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -413,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -422,12 +434,12 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>title</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>description</t>
         </is>
@@ -436,36 +448,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Einführung in digitale Lehre</t>
+          <t>Designing Effective Moodle Courses for Higher Education</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>In diesem Seminar lernen Sie die Grundlagen digitaler Lehrformate kennen. Themen: Lernplattformen, Videokonferenzen, digitale Prüfungsformate. Zielgruppe: Dozierende aller Fachrichtungen.</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Workshop: Aktivierende Methoden in der Hochschullehre</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Praktischer Workshop zu Methoden, die Studierende aktiv einbinden. Arbeit in Kleingruppen, Erprobung von Techniken. Angebot der Hochschuldidaktik.</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Coaching für neue Dozierende</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Individuelle Beratung und Begleitung für neue Lehrende. Reflexion der eigenen Lehrpraxis, kollegialer Austausch. Einzelcoaching oder Kleingruppen.</t>
+          <t>This professional development course supports higher education teachers in designing, structuring, and implementing pedagogically sound Moodle courses. Participants will learn how to translate didactic concepts into functional Moodle environments that support student engagement, self-regulated learning, and assessment.
+The course combines instructional design principles with hands-on practice in Moodle. Participants will explore core Moodle functionalities (e.g., activities, resources, assessments, feedback, and analytics) and learn how to align them with learning objectives, constructive alignment, and evidence-based teaching strategies.
+By the end of the course, participants will have developed a prototype Moodle course or a redesigned course unit that is ready for implementation in their own teaching context.</t>
         </is>
       </c>
     </row>

</xml_diff>